<commit_message>
Adds scripts for benchmark characterization and final results
</commit_message>
<xml_diff>
--- a/executionComparison.xlsx
+++ b/executionComparison.xlsx
@@ -557,12 +557,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -888,23 +891,26 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
@@ -919,6 +925,7 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -937,9 +944,7 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -1256,7 +1261,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="B2:C2"/>

</xml_diff>